<commit_message>
adding _config.yaml for GitHub pages, edits to table
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke.thompson/git/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914BB360-7EAF-F742-BCA1-D8D7C37B0E9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9059EE7F-C965-5045-A9A3-FB3BB3B36FDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="18240" windowWidth="32000" windowHeight="17760" xr2:uid="{57040ACB-952F-4E4F-A09F-4435F81F22CE}"/>
   </bookViews>
@@ -63,18 +63,12 @@
     <t>DNA</t>
   </si>
   <si>
-    <t>Metabarcoding</t>
-  </si>
-  <si>
     <t>erie</t>
   </si>
   <si>
     <t>Goodwin</t>
   </si>
   <si>
-    <t>Metabarcoding, Metagenomics</t>
-  </si>
-  <si>
     <t>BioProject</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>[PRJNA702128](https://www.ncbi.nlm.nih.gov/bioproject/PRJNA702128)</t>
+  </si>
+  <si>
+    <t>metabarcoding</t>
+  </si>
+  <si>
+    <t>metabarcoding, metagenomics</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:G4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,10 +478,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -498,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>31</v>
@@ -506,25 +506,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>149</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>